<commit_message>
slightly modified spreadsheet structure, no changes to data
</commit_message>
<xml_diff>
--- a/data/arabidopsis.xlsx
+++ b/data/arabidopsis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.rodriguez\Documents\github\CoVOCom\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.rodriguez\Documents\positron-git\CoVOCom\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96379FB3-01D3-4EF4-9020-6DE29C5F0740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF3FB9E-C848-4A46-87FD-3242ED2B3092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -933,23 +936,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E142" workbookViewId="0">
-      <selection activeCell="J164" sqref="J164"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="29" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>